<commit_message>
Incluído um script r e mais uma aba na planilha
Estávamos usando o teste errado, por isso não estávamos obtendo o mesmo
resultado. Não podemos usar o teste binomial.
</commit_message>
<xml_diff>
--- a/util/bernoulli-confidence-interval.xlsx
+++ b/util/bernoulli-confidence-interval.xlsx
@@ -9,10 +9,11 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="12240" windowHeight="6156"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="12240" windowHeight="6156" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="intervalo de confiança" sheetId="1" r:id="rId1"/>
+    <sheet name="teste de hipótese" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="152511"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="38">
   <si>
     <t>S=</t>
   </si>
@@ -66,16 +67,90 @@
   </si>
   <si>
     <t>]</t>
+  </si>
+  <si>
+    <t>h0</t>
+  </si>
+  <si>
+    <t>(h0-p)</t>
+  </si>
+  <si>
+    <t>Z score:</t>
+  </si>
+  <si>
+    <t>Dado a população real, a chance que exista uma média menor ou igual a média de h0 é de:</t>
+  </si>
+  <si>
+    <t>p-value=</t>
+  </si>
+  <si>
+    <t>(tentar obter um p-value menor que 0.05)</t>
+  </si>
+  <si>
+    <t>(tentar obter um hipótese maior que .6)</t>
+  </si>
+  <si>
+    <t>One-tail-test</t>
+  </si>
+  <si>
+    <t>sucesso(p)</t>
+  </si>
+  <si>
+    <t>n</t>
+  </si>
+  <si>
+    <t>hipótese (ph0)</t>
+  </si>
+  <si>
+    <t>Amostra da hipótese</t>
+  </si>
+  <si>
+    <t>média</t>
+  </si>
+  <si>
+    <t>População</t>
+  </si>
+  <si>
+    <t>Sh0</t>
+  </si>
+  <si>
+    <t>Spop.=</t>
+  </si>
+  <si>
+    <t>Z-score</t>
+  </si>
+  <si>
+    <t>Média (pop)</t>
+  </si>
+  <si>
+    <t>p-value</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> (greater)</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> (lesser)</t>
+  </si>
+  <si>
+    <t>Confidence</t>
+  </si>
+  <si>
+    <t>Interval</t>
+  </si>
+  <si>
+    <t>z-score (critical value)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="1">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="0.0%"/>
+    <numFmt numFmtId="165" formatCode="0.000%"/>
+    <numFmt numFmtId="206" formatCode="0.000"/>
   </numFmts>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -90,8 +165,38 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="4" tint="-0.499984740745262"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -101,6 +206,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF00B0F0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -118,10 +229,20 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="206" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -403,88 +524,131 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:E14"/>
+  <dimension ref="A2:H14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="5.5546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>6</v>
       </c>
       <c r="B2" s="2">
+        <v>32</v>
+      </c>
+      <c r="D2" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E2" s="2">
+        <v>0.6</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>7</v>
       </c>
       <c r="B3" s="2">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+        <v>8</v>
+      </c>
+      <c r="D3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E3">
+        <f>B5-E2</f>
+        <v>0.20000000000000007</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>1</v>
       </c>
       <c r="B4">
         <f>B2+B3</f>
-        <v>24</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+        <v>40</v>
+      </c>
+      <c r="D4" t="s">
+        <v>16</v>
+      </c>
+      <c r="E4">
+        <f>E3/B10</f>
+        <v>3.1224989991992</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>2</v>
       </c>
       <c r="B5">
         <f>(B3*0+B2*1)/B4</f>
-        <v>0.58333333333333337</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+        <v>0.8</v>
+      </c>
+      <c r="D5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>3</v>
       </c>
       <c r="B6">
         <f>1-B5</f>
-        <v>0.41666666666666663</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+        <v>0.19999999999999996</v>
+      </c>
+      <c r="E6" s="3">
+        <f>1-_xlfn.NORM.S.DIST(E4,TRUE)</f>
+        <v>8.9661357592507596E-4</v>
+      </c>
+      <c r="F6" t="s">
+        <v>18</v>
+      </c>
+      <c r="G6" s="4">
+        <f>E6</f>
+        <v>8.9661357592507596E-4</v>
+      </c>
+      <c r="H6" s="5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>4</v>
       </c>
       <c r="B7">
         <f>(B3*POWER(0-B5,2)+B2*POWER(1-B5,2))/(B4-1)</f>
-        <v>0.25362318840579712</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+        <v>0.1641025641025641</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>0</v>
       </c>
       <c r="B8">
         <f>SQRT(B7)</f>
-        <v>0.50361015518533492</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+        <v>0.40509574683346666</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>5</v>
       </c>
       <c r="B10">
         <f>B8/SQRT(B4)</f>
-        <v>0.10279899245732688</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+        <v>6.4051261522034858E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="C11" t="s">
         <v>11</v>
       </c>
@@ -495,7 +659,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>8</v>
       </c>
@@ -504,18 +668,18 @@
       </c>
       <c r="C12">
         <f>$B$10*1</f>
-        <v>0.10279899245732688</v>
+        <v>6.4051261522034858E-2</v>
       </c>
       <c r="D12">
         <f>$B$5-C12</f>
-        <v>0.48053434087600649</v>
+        <v>0.73594873847796516</v>
       </c>
       <c r="E12">
         <f>$B$5+C12</f>
-        <v>0.68613232579066019</v>
-      </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+        <v>0.86405126152203493</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>9</v>
       </c>
@@ -524,18 +688,18 @@
       </c>
       <c r="C13">
         <f>$B$10*2</f>
-        <v>0.20559798491465375</v>
+        <v>0.12810252304406972</v>
       </c>
       <c r="D13">
         <f>$B$5-C13</f>
-        <v>0.37773534841867962</v>
+        <v>0.67189747695593027</v>
       </c>
       <c r="E13">
         <f>$B$5+C13</f>
-        <v>0.78893131824798712</v>
-      </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+        <v>0.92810252304406982</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>10</v>
       </c>
@@ -544,18 +708,220 @@
       </c>
       <c r="C14">
         <f>$B$10*3</f>
-        <v>0.30839697737198063</v>
+        <v>0.19215378456610457</v>
       </c>
       <c r="D14">
         <f>$B$5-C14</f>
-        <v>0.27493635596135274</v>
+        <v>0.6078462154338955</v>
       </c>
       <c r="E14">
         <f>$B$5+C14</f>
-        <v>0.89173031070531406</v>
+        <v>0.99215378456610459</v>
       </c>
     </row>
   </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F16"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.77734375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.21875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.88671875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B2" s="10">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B3" s="10">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B4" s="10">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>25</v>
+      </c>
+      <c r="D6" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>26</v>
+      </c>
+      <c r="B7">
+        <f>B4</f>
+        <v>0.6</v>
+      </c>
+      <c r="D7" t="s">
+        <v>29</v>
+      </c>
+      <c r="E7">
+        <f>B8/SQRT(B3)</f>
+        <v>7.7459666924148324E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>28</v>
+      </c>
+      <c r="B8">
+        <f>SQRT(B7*(1-B7))</f>
+        <v>0.4898979485566356</v>
+      </c>
+      <c r="D8" t="s">
+        <v>31</v>
+      </c>
+      <c r="E8">
+        <f>B2/B3</f>
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="D9" t="s">
+        <v>30</v>
+      </c>
+      <c r="E9">
+        <f>(E8-B7)/E7</f>
+        <v>2.5819888974716125</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="D10" t="s">
+        <v>32</v>
+      </c>
+      <c r="E10" s="8">
+        <f>1-_xlfn.NORM.S.DIST(E9,TRUE)</f>
+        <v>4.9116372537596487E-3</v>
+      </c>
+      <c r="F10" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E11">
+        <f>1-E10</f>
+        <v>0.99508836274624035</v>
+      </c>
+      <c r="F11" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>35</v>
+      </c>
+      <c r="B13" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="C13" s="7"/>
+      <c r="D13" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="E13" s="7"/>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <v>0.95</v>
+      </c>
+      <c r="B14" s="9">
+        <f>_xlfn.NORM.S.INV(A14)</f>
+        <v>1.6448536269514715</v>
+      </c>
+      <c r="C14">
+        <f>$E$7*B14</f>
+        <v>0.1274098140826383</v>
+      </c>
+      <c r="D14" s="6">
+        <f>$E$8-C14</f>
+        <v>0.67259018591736175</v>
+      </c>
+      <c r="E14" s="6">
+        <f>$E$8+C14</f>
+        <v>0.92740981408263834</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A15">
+        <v>0.97</v>
+      </c>
+      <c r="B15" s="9">
+        <f t="shared" ref="B15:B16" si="0">_xlfn.NORM.S.INV(A15)</f>
+        <v>1.8807936081512504</v>
+      </c>
+      <c r="C15">
+        <f t="shared" ref="C15:C16" si="1">$E$7*B15</f>
+        <v>0.145685646440463</v>
+      </c>
+      <c r="D15" s="6">
+        <f t="shared" ref="D15:D16" si="2">$E$8-C15</f>
+        <v>0.65431435355953704</v>
+      </c>
+      <c r="E15" s="6">
+        <f t="shared" ref="E15:E16" si="3">$E$8+C15</f>
+        <v>0.94568564644046305</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A16">
+        <v>0.99</v>
+      </c>
+      <c r="B16" s="9">
+        <f t="shared" si="0"/>
+        <v>2.3263478740408408</v>
+      </c>
+      <c r="C16">
+        <f t="shared" si="1"/>
+        <v>0.18019813147290409</v>
+      </c>
+      <c r="D16" s="6">
+        <f t="shared" si="2"/>
+        <v>0.61980186852709596</v>
+      </c>
+      <c r="E16" s="6">
+        <f t="shared" si="3"/>
+        <v>0.98019813147290413</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="D13:E13"/>
+    <mergeCell ref="B13:C13"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>